<commit_message>
not preload owl vit model anymore
</commit_message>
<xml_diff>
--- a/output/excel/single_Ghost Rider 4S1P ATL CosMX HPT RS 20HK2 BSMI LOA.xlsx
+++ b/output/excel/single_Ghost Rider 4S1P ATL CosMX HPT RS 20HK2 BSMI LOA.xlsx
@@ -459,7 +459,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Page 1 (loc: cropped_image:model_name.png): "型式：20HK2"</t>
+          <t>Page 1 (loc: cropped_image:model_name.png): "型式: 20HK2"</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>頁碼採絕對 1-based。本文件主要語言為中文。僅 model_name 有切圖並成功辨識，其他欄位在切圖與 hints 搜尋均未獲值。</t>
+          <t>主要語言為中文。僅 model_name 有切圖且成功辨識，其他欄位在切圖與 hints 搜尋均未獲值。頁碼採絕對 1-based。</t>
         </is>
       </c>
     </row>

</xml_diff>